<commit_message>
ch-elm with version 1.1.1
</commit_message>
<xml_diff>
--- a/ig/ch-elm/CodeSystem-ch-elm-foph-business-rules.xlsx
+++ b/ig/ch-elm/CodeSystem-ch-elm-foph-business-rules.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>1.1.0</t>
+    <t>1.1.1</t>
   </si>
   <si>
     <t>Name</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-01-31T12:59:55+01:00</t>
+    <t>2024-02-27T13:26:20+01:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>

<commit_message>
ch-elm with version 1.2.0
</commit_message>
<xml_diff>
--- a/ig/ch-elm/CodeSystem-ch-elm-foph-business-rules.xlsx
+++ b/ig/ch-elm/CodeSystem-ch-elm-foph-business-rules.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="78">
   <si>
     <t>Property</t>
   </si>
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>1.1.1</t>
+    <t>1.2.0</t>
   </si>
   <si>
     <t>Name</t>
@@ -42,7 +42,7 @@
     <t>Title</t>
   </si>
   <si>
-    <t>CH ELM Foph Business Rules</t>
+    <t>CH ELM FOPH Business Rules</t>
   </si>
   <si>
     <t>Status</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-02-27T13:26:20+01:00</t>
+    <t>2024-03-28T10:46:20+01:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -150,6 +150,15 @@
     <t>A purely informational message.</t>
   </si>
   <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>FOPH-000</t>
+  </si>
+  <si>
+    <t>Generic Information</t>
+  </si>
+  <si>
     <t>warning</t>
   </si>
   <si>
@@ -159,10 +168,31 @@
     <t>If the rule is violated, the resource is conformant, but it is not necessarily following best practice.</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>FOPH-003</t>
+    <t>FOPH-005</t>
+  </si>
+  <si>
+    <t>The required anonymization for the reported organism was violated. The following field(s) are affected: %fields%</t>
+  </si>
+  <si>
+    <t>FOPH-011</t>
+  </si>
+  <si>
+    <t>The material is already specified by the leading code. The additional material specified in specimen.type will be ignored.</t>
+  </si>
+  <si>
+    <t>FOPH-010</t>
+  </si>
+  <si>
+    <t>Attention, the code %code% (%codeSystem%) expires on %validTo%. Please adjust your systems by this date.</t>
+  </si>
+  <si>
+    <t>FOPH-001</t>
+  </si>
+  <si>
+    <t>Generic Warning</t>
+  </si>
+  <si>
+    <t>FOPH-006</t>
   </si>
   <si>
     <t>The following elements for the patient's address are expected: %missingElements%.</t>
@@ -177,16 +207,46 @@
     <t>If the rule is violated, the resource is not conformant.</t>
   </si>
   <si>
-    <t>FOPH-001</t>
-  </si>
-  <si>
-    <t>The provided laboratory identification %identifier% is either unknown or corresponds to a laboratory for which your account does not have reporting permissions. Please verify your laboratory identification. If it's correct, complete the necessary onboarding process before submitting data on behalf of this lab.</t>
+    <t>FOPH-009</t>
+  </si>
+  <si>
+    <t>The transmitted code %code% (%codeSystem%) is outside the defined validity period %validFrom% - %validTo%.</t>
   </si>
   <si>
     <t>FOPH-002</t>
   </si>
   <si>
-    <t>The required anonymization for the reported organism was violated.</t>
+    <t>Generic Error</t>
+  </si>
+  <si>
+    <t>FOPH-007</t>
+  </si>
+  <si>
+    <t>The specified material is not supported by the provided leading code.</t>
+  </si>
+  <si>
+    <t>FOPH-012</t>
+  </si>
+  <si>
+    <t>The transmitted leading code %code% (%codeSystem%) could not be found in the current value set.</t>
+  </si>
+  <si>
+    <t>FOPH-008</t>
+  </si>
+  <si>
+    <t>The specified organism is not supported by the provided leading code.</t>
+  </si>
+  <si>
+    <t>FOPH-004</t>
+  </si>
+  <si>
+    <t>The provided laboratory identification "%identifier%" is either unknown or corresponds to a laboratory for which your account does not have reporting permissions. Please verify your laboratory identification. If it's correct, complete the necessary onboarding process before submitting data on behalf of this lab.</t>
+  </si>
+  <si>
+    <t>FOPH-013</t>
+  </si>
+  <si>
+    <t>The transmitted code %code% (%codeSystem%) is outside the defined validity period.</t>
   </si>
 </sst>
 </file>
@@ -501,7 +561,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -537,33 +597,33 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C3" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="D3" t="s" s="2">
         <v>47</v>
       </c>
+      <c r="D3" s="2"/>
     </row>
     <row r="4">
       <c r="A4" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="B4" t="s" s="2">
         <v>48</v>
       </c>
-      <c r="B4" t="s" s="2">
+      <c r="C4" t="s" s="2">
         <v>49</v>
       </c>
-      <c r="C4" t="s" s="2">
+      <c r="D4" t="s" s="2">
         <v>50</v>
       </c>
-      <c r="D4" s="2"/>
     </row>
     <row r="5">
       <c r="A5" t="s" s="2">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B5" t="s" s="2">
         <v>51</v>
@@ -571,33 +631,153 @@
       <c r="C5" t="s" s="2">
         <v>52</v>
       </c>
-      <c r="D5" t="s" s="2">
-        <v>53</v>
-      </c>
+      <c r="D5" s="2"/>
     </row>
     <row r="6">
       <c r="A6" t="s" s="2">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B6" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="C6" t="s" s="2">
         <v>54</v>
-      </c>
-      <c r="C6" t="s" s="2">
-        <v>55</v>
       </c>
       <c r="D6" s="2"/>
     </row>
     <row r="7">
       <c r="A7" t="s" s="2">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B7" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="C7" t="s" s="2">
         <v>56</v>
       </c>
-      <c r="C7" t="s" s="2">
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="B8" t="s" s="2">
         <v>57</v>
       </c>
-      <c r="D7" s="2"/>
+      <c r="C8" t="s" s="2">
+        <v>58</v>
+      </c>
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="B9" t="s" s="2">
+        <v>59</v>
+      </c>
+      <c r="C9" t="s" s="2">
+        <v>60</v>
+      </c>
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="B10" t="s" s="2">
+        <v>61</v>
+      </c>
+      <c r="C10" t="s" s="2">
+        <v>62</v>
+      </c>
+      <c r="D10" t="s" s="2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="B11" t="s" s="2">
+        <v>64</v>
+      </c>
+      <c r="C11" t="s" s="2">
+        <v>65</v>
+      </c>
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="B12" t="s" s="2">
+        <v>66</v>
+      </c>
+      <c r="C12" t="s" s="2">
+        <v>67</v>
+      </c>
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="B13" t="s" s="2">
+        <v>68</v>
+      </c>
+      <c r="C13" t="s" s="2">
+        <v>69</v>
+      </c>
+      <c r="D13" s="2"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="B14" t="s" s="2">
+        <v>70</v>
+      </c>
+      <c r="C14" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="B15" t="s" s="2">
+        <v>72</v>
+      </c>
+      <c r="C15" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="D15" s="2"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="B16" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="C16" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="D16" s="2"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="B17" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="C17" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="D17" s="2"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>